<commit_message>
Added more realistic sample data
</commit_message>
<xml_diff>
--- a/Example Data/prizes.xlsx
+++ b/Example Data/prizes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="460" windowWidth="27700" windowHeight="17540"/>
+    <workbookView xWindow="1220" yWindow="460" windowWidth="27580" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
   <si>
     <t>Prize Name</t>
   </si>
@@ -41,137 +41,203 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Gold Favor Ring</t>
-  </si>
-  <si>
-    <t>Silver Ring</t>
-  </si>
-  <si>
-    <t>The Eolian Wooden Sign</t>
-  </si>
-  <si>
-    <t>Game of Thrones Dragon Egg Canister</t>
-  </si>
-  <si>
-    <t>Game of Thrones House Sigil Wine Charms</t>
-  </si>
-  <si>
-    <t>Game of Thrones Ceramic Steins</t>
-  </si>
-  <si>
-    <t>Executive Knight Pen Holder</t>
-  </si>
-  <si>
-    <t>Freedom of the Mask</t>
-  </si>
-  <si>
     <t>Book</t>
   </si>
   <si>
-    <t>Down and Out in Purgatory</t>
-  </si>
-  <si>
-    <t>The Burglar Who Counted the Spoons</t>
-  </si>
-  <si>
-    <t>The Authentic William James</t>
-  </si>
-  <si>
-    <t>Shades of London series by Maureen Johnson</t>
-  </si>
-  <si>
-    <t>Vacations from Hell anthology</t>
-  </si>
-  <si>
-    <t>The Last Little Blue Envelope by Maureen Johnson</t>
-  </si>
-  <si>
-    <t>Razor's Edge by Martha Wells</t>
-  </si>
-  <si>
-    <t>The Fall of Ile-Rien series by Martha Wells</t>
-  </si>
-  <si>
-    <t>Promise of Blood &amp; In the Field Marshal's Shadow by Brian McClellan</t>
-  </si>
-  <si>
-    <t>Purloined Poodle by Kevin Hearne, trade edition</t>
-  </si>
-  <si>
-    <t>Kurt Cobain and Mozart are both Dead</t>
-  </si>
-  <si>
     <t>Comic</t>
   </si>
   <si>
-    <t>Fifth Beatle limited edition</t>
-  </si>
-  <si>
-    <t>Fight Club 2</t>
-  </si>
-  <si>
-    <t>Buffy Season Eight Vol 1</t>
-  </si>
-  <si>
-    <t>Archives Tales from the Crypt</t>
-  </si>
-  <si>
-    <t>Mansions of Madness Second Edition</t>
-  </si>
-  <si>
     <t>Game</t>
   </si>
   <si>
-    <t>Runebound</t>
-  </si>
-  <si>
-    <t>Twilight Imperium</t>
-  </si>
-  <si>
-    <t>Catan - Traveler</t>
-  </si>
-  <si>
-    <t>Crusaders of the Lost Idols + DLC</t>
-  </si>
-  <si>
-    <t>Johari</t>
-  </si>
-  <si>
-    <t>Temeraire Medallion</t>
-  </si>
-  <si>
     <t>Jewelry</t>
   </si>
   <si>
-    <t>Lizzie Borden's Axe Pendant</t>
-  </si>
-  <si>
-    <t>Khovura Medallion</t>
-  </si>
-  <si>
-    <t>Wheel of Time Money Clip</t>
-  </si>
-  <si>
-    <t>Powder Keg pin</t>
-  </si>
-  <si>
-    <t>Smaug the Golden Necklace</t>
-  </si>
-  <si>
-    <t>JoCo Cabin</t>
-  </si>
-  <si>
     <t>JoCo</t>
   </si>
   <si>
     <t>Misc</t>
+  </si>
+  <si>
+    <t>Comic 1</t>
+  </si>
+  <si>
+    <t>JoCo 2</t>
+  </si>
+  <si>
+    <t>Comic 3</t>
+  </si>
+  <si>
+    <t>Jewelry 4</t>
+  </si>
+  <si>
+    <t>Book 5</t>
+  </si>
+  <si>
+    <t>Game 6</t>
+  </si>
+  <si>
+    <t>JoCo 7</t>
+  </si>
+  <si>
+    <t>Misc 8</t>
+  </si>
+  <si>
+    <t>Comic 9</t>
+  </si>
+  <si>
+    <t>Jewelry 10</t>
+  </si>
+  <si>
+    <t>Jewelry 11</t>
+  </si>
+  <si>
+    <t>Misc 12</t>
+  </si>
+  <si>
+    <t>Comic 13</t>
+  </si>
+  <si>
+    <t>Jewelry 14</t>
+  </si>
+  <si>
+    <t>Comic 15</t>
+  </si>
+  <si>
+    <t>Game 16</t>
+  </si>
+  <si>
+    <t>Game 17</t>
+  </si>
+  <si>
+    <t>Book 18</t>
+  </si>
+  <si>
+    <t>Misc 19</t>
+  </si>
+  <si>
+    <t>JoCo 20</t>
+  </si>
+  <si>
+    <t>Comic 21</t>
+  </si>
+  <si>
+    <t>Book 22</t>
+  </si>
+  <si>
+    <t>Comic 23</t>
+  </si>
+  <si>
+    <t>Comic 24</t>
+  </si>
+  <si>
+    <t>Jewelry 25</t>
+  </si>
+  <si>
+    <t>Book 26</t>
+  </si>
+  <si>
+    <t>Misc 27</t>
+  </si>
+  <si>
+    <t>Jewelry 28</t>
+  </si>
+  <si>
+    <t>Book 29</t>
+  </si>
+  <si>
+    <t>Game 30</t>
+  </si>
+  <si>
+    <t>Book 31</t>
+  </si>
+  <si>
+    <t>JoCo 32</t>
+  </si>
+  <si>
+    <t>Game 33</t>
+  </si>
+  <si>
+    <t>Jewelry 34</t>
+  </si>
+  <si>
+    <t>Jewelry 35</t>
+  </si>
+  <si>
+    <t>JoCo 36</t>
+  </si>
+  <si>
+    <t>Misc 37</t>
+  </si>
+  <si>
+    <t>Game 38</t>
+  </si>
+  <si>
+    <t>Misc 39</t>
+  </si>
+  <si>
+    <t>Comic 40</t>
+  </si>
+  <si>
+    <t>Misc 41</t>
+  </si>
+  <si>
+    <t>Book 42</t>
+  </si>
+  <si>
+    <t>Misc 43</t>
+  </si>
+  <si>
+    <t>Jewelry 44</t>
+  </si>
+  <si>
+    <t>Comic 45</t>
+  </si>
+  <si>
+    <t>Misc 46</t>
+  </si>
+  <si>
+    <t>Book 47</t>
+  </si>
+  <si>
+    <t>JoCo 48</t>
+  </si>
+  <si>
+    <t>Jewelry 49</t>
+  </si>
+  <si>
+    <t>Comic 50</t>
+  </si>
+  <si>
+    <t>Comic 51</t>
+  </si>
+  <si>
+    <t>Game 52</t>
+  </si>
+  <si>
+    <t>Comic 53</t>
+  </si>
+  <si>
+    <t>JoCo 54</t>
+  </si>
+  <si>
+    <t>Game 55</t>
+  </si>
+  <si>
+    <t>JoCo 56</t>
+  </si>
+  <si>
+    <t>Comic 57</t>
+  </si>
+  <si>
+    <t>Misc 58</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +261,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -213,7 +285,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -221,17 +293,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -510,18 +587,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,400 +611,647 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>364</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="G2">
+        <f>SUM(B:B)</f>
+        <v>16167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>349</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>298</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>365</v>
+      </c>
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>254</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>302</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>339</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>165</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>185</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>391</v>
+      </c>
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>482</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>300</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>256</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>407</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>460</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>486</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>355</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B26">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
         <v>6</v>
-      </c>
-      <c r="C26" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B27">
-        <v>6</v>
+        <v>236</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>161</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>295</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>290</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>486</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>436</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>328</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>177</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>277</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39">
+        <v>402</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40">
+        <v>489</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41">
+        <v>287</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42">
+        <v>486</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43">
+        <v>144</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44">
+        <v>474</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45">
+        <v>329</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46">
+        <v>436</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47">
+        <v>484</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48">
+        <v>238</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49">
+        <v>55</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50">
+        <v>298</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51">
+        <v>390</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52">
+        <v>344</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53">
+        <v>204</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54">
+        <v>41</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55">
+        <v>131</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56">
+        <v>462</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57">
+        <v>229</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58">
+        <v>309</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59">
+        <v>408</v>
+      </c>
+      <c r="C59" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>